<commit_message>
Small fix to excel file and sql
</commit_message>
<xml_diff>
--- a/ExcelFiles/IncomeReports.xlsx
+++ b/ExcelFiles/IncomeReports.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,6 +72,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Excursion"/>
+    <tableColumn id="2" name="Income"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,12 +375,15 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="10.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,5 +393,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>